<commit_message>
Added Skill feature testcases
</commit_message>
<xml_diff>
--- a/Project Mars Test Condition and Test Cases.xlsx
+++ b/Project Mars Test Condition and Test Cases.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/milan/Documents/Project Mars/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{143ADC57-0978-3740-97F6-105A1242F820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1970896A-2EB6-D74D-9540-EF0E88C83520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" activeTab="1" xr2:uid="{721A54BA-CEF9-8143-A086-0510A3CE7201}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" activeTab="2" xr2:uid="{721A54BA-CEF9-8143-A086-0510A3CE7201}"/>
   </bookViews>
   <sheets>
     <sheet name="Profile Page Test Scenarios" sheetId="5" r:id="rId1"/>
     <sheet name="language Test Cases" sheetId="4" r:id="rId2"/>
+    <sheet name="Skill Test Cases" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="160">
   <si>
     <t>ID</t>
   </si>
@@ -931,6 +932,143 @@
   </si>
   <si>
     <t>4.User should not able to see "Add New" button.</t>
+  </si>
+  <si>
+    <t>Verify that if the user is able to click  on Skill Tab.</t>
+  </si>
+  <si>
+    <t>3.User should be able to navigate to Skill Tab.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Step 3:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Click on "Skill" Tab</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify the "Add New" button is visible for the the Skill Tab.</t>
+  </si>
+  <si>
+    <t>3.User should be able to navigate Skill Tab.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Verify the "Add"and "Cancle" button is visible for the the Skill Tab.</t>
+  </si>
+  <si>
+    <t>Verify that if user can successfully enter the value for "Add Skill" textbox.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Step 4: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Eneter the value in "Add Skill" textbox.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> Verify that user can successfully add Skill to a list using "Add" button.</t>
+  </si>
+  <si>
+    <t>7.User should be able to see new skill added in list.</t>
+  </si>
+  <si>
+    <t>Verify that user gets notification when successfully add Skill.</t>
+  </si>
+  <si>
+    <t>7.Notification "Communication has been added to your Skill" should be displayed</t>
+  </si>
+  <si>
+    <t>TextBox:Communication</t>
+  </si>
+  <si>
+    <t>Dropdown:Begginer</t>
+  </si>
+  <si>
+    <t>Verify that user gets notification when  "Add Skill" textbox left blank.</t>
+  </si>
+  <si>
+    <t>5.Notification "Please enter Skill and level" should be displayed.</t>
+  </si>
+  <si>
+    <t>4.User should be able to see "Update" and "Cancel" button.</t>
+  </si>
+  <si>
+    <t>Verify that user can successfully Update Skill using "Update" button.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Step 3:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Click on "skill" Tab</t>
+    </r>
+  </si>
+  <si>
+    <t>TextBox:Cooking</t>
+  </si>
+  <si>
+    <t>Dropdown:Beginner</t>
+  </si>
+  <si>
+    <t>Verify that user gets notification when successfully Update Skill.</t>
+  </si>
+  <si>
+    <t>7.Notification "Cooking has been updated to your language" should be displayed</t>
+  </si>
+  <si>
+    <t>Verify that user is able to delete Skill using delete button.</t>
+  </si>
+  <si>
+    <t>7.Notification " This Skill is already exist in Skill list"should be displayed.</t>
+  </si>
+  <si>
+    <t>Verify that user gets notification when successfully delete Skill.</t>
+  </si>
+  <si>
+    <t>4.Notification "Cooking has been deleted to your Skill" should be displayed</t>
   </si>
 </sst>
 </file>
@@ -1041,13 +1179,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1626,7 +1764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD8AB10B-E452-264E-9895-BDC2268876B3}">
   <dimension ref="A1:I158"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+    <sheetView topLeftCell="A173" zoomScale="90" workbookViewId="0">
       <selection sqref="A1:J163"/>
     </sheetView>
   </sheetViews>
@@ -1676,7 +1814,7 @@
       <c r="B2" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="9" t="s">
         <v>52</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -1686,7 +1824,7 @@
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B3" s="5"/>
       <c r="C3" s="7"/>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="8" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1706,7 +1844,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" s="5"/>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="6" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1724,7 +1862,7 @@
       <c r="B9" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="9" t="s">
         <v>52</v>
       </c>
       <c r="E9" s="2" t="s">
@@ -1734,7 +1872,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B10" s="5"/>
       <c r="C10" s="7"/>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="8" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1754,7 +1892,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13" s="5"/>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="6" t="s">
         <v>54</v>
       </c>
       <c r="E13" t="s">
@@ -1778,7 +1916,7 @@
       <c r="B17" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="9" t="s">
         <v>52</v>
       </c>
       <c r="E17" s="2" t="s">
@@ -1788,7 +1926,7 @@
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B18" s="5"/>
       <c r="C18" s="7"/>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="8" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1808,7 +1946,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B21" s="5"/>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="6" t="s">
         <v>54</v>
       </c>
       <c r="E21" t="s">
@@ -1841,7 +1979,7 @@
       <c r="B26" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="9" t="s">
         <v>52</v>
       </c>
       <c r="E26" s="2" t="s">
@@ -1851,7 +1989,7 @@
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B27" s="5"/>
       <c r="C27" s="7"/>
-      <c r="E27" s="6" t="s">
+      <c r="E27" s="8" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1871,7 +2009,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B30" s="5"/>
-      <c r="C30" s="9" t="s">
+      <c r="C30" s="6" t="s">
         <v>54</v>
       </c>
       <c r="E30" t="s">
@@ -1903,7 +2041,7 @@
       <c r="B35" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="9" t="s">
         <v>52</v>
       </c>
       <c r="E35" s="2" t="s">
@@ -1913,7 +2051,7 @@
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B36" s="5"/>
       <c r="C36" s="7"/>
-      <c r="E36" s="6" t="s">
+      <c r="E36" s="8" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1933,7 +2071,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B39" s="5"/>
-      <c r="C39" s="9" t="s">
+      <c r="C39" s="6" t="s">
         <v>54</v>
       </c>
       <c r="E39" t="s">
@@ -1966,7 +2104,7 @@
       <c r="B44" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="C44" s="9" t="s">
         <v>52</v>
       </c>
       <c r="E44" s="2" t="s">
@@ -1976,7 +2114,7 @@
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B45" s="5"/>
       <c r="C45" s="7"/>
-      <c r="E45" s="6" t="s">
+      <c r="E45" s="8" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1996,7 +2134,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B48" s="5"/>
-      <c r="C48" s="9" t="s">
+      <c r="C48" s="6" t="s">
         <v>54</v>
       </c>
       <c r="E48" t="s">
@@ -2047,7 +2185,7 @@
       <c r="B55" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="C55" s="8" t="s">
+      <c r="C55" s="9" t="s">
         <v>52</v>
       </c>
       <c r="E55" s="2" t="s">
@@ -2057,7 +2195,7 @@
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B56" s="11"/>
       <c r="C56" s="7"/>
-      <c r="E56" s="6" t="s">
+      <c r="E56" s="8" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2077,7 +2215,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B59" s="11"/>
-      <c r="C59" s="9" t="s">
+      <c r="C59" s="6" t="s">
         <v>54</v>
       </c>
       <c r="E59" t="s">
@@ -2115,10 +2253,10 @@
       <c r="B64" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C64" s="8" t="s">
+      <c r="C64" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="E64" s="6" t="s">
+      <c r="E64" s="8" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2145,7 +2283,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B68" s="5"/>
-      <c r="C68" s="9" t="s">
+      <c r="C68" s="6" t="s">
         <v>54</v>
       </c>
       <c r="E68" t="s">
@@ -2199,7 +2337,7 @@
       <c r="B75" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C75" s="8" t="s">
+      <c r="C75" s="9" t="s">
         <v>52</v>
       </c>
       <c r="E75" s="2" t="s">
@@ -2209,7 +2347,7 @@
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B76" s="5"/>
       <c r="C76" s="7"/>
-      <c r="E76" s="6" t="s">
+      <c r="E76" s="8" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2229,7 +2367,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B79" s="5"/>
-      <c r="C79" s="9" t="s">
+      <c r="C79" s="6" t="s">
         <v>54</v>
       </c>
       <c r="E79" t="s">
@@ -2262,7 +2400,7 @@
       <c r="B84" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C84" s="8" t="s">
+      <c r="C84" s="9" t="s">
         <v>52</v>
       </c>
       <c r="E84" s="2" t="s">
@@ -2272,7 +2410,7 @@
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B85" s="5"/>
       <c r="C85" s="7"/>
-      <c r="E85" s="6" t="s">
+      <c r="E85" s="8" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2292,7 +2430,7 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B88" s="5"/>
-      <c r="C88" s="9" t="s">
+      <c r="C88" s="6" t="s">
         <v>54</v>
       </c>
       <c r="E88" t="s">
@@ -2325,7 +2463,7 @@
       <c r="B94" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C94" s="8" t="s">
+      <c r="C94" s="9" t="s">
         <v>52</v>
       </c>
       <c r="E94" s="2" t="s">
@@ -2335,7 +2473,7 @@
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B95" s="5"/>
       <c r="C95" s="7"/>
-      <c r="E95" s="6" t="s">
+      <c r="E95" s="8" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2355,7 +2493,7 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B98" s="5"/>
-      <c r="C98" s="9" t="s">
+      <c r="C98" s="6" t="s">
         <v>54</v>
       </c>
       <c r="E98" t="s">
@@ -2368,7 +2506,7 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B100" s="5"/>
-      <c r="C100" s="9" t="s">
+      <c r="C100" s="6" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2383,7 +2521,7 @@
       <c r="B103" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="C103" s="8" t="s">
+      <c r="C103" s="9" t="s">
         <v>52</v>
       </c>
       <c r="E103" s="2" t="s">
@@ -2393,7 +2531,7 @@
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B104" s="5"/>
       <c r="C104" s="7"/>
-      <c r="E104" s="6" t="s">
+      <c r="E104" s="8" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2413,7 +2551,7 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B107" s="5"/>
-      <c r="C107" s="9" t="s">
+      <c r="C107" s="6" t="s">
         <v>54</v>
       </c>
       <c r="E107" t="s">
@@ -2470,7 +2608,7 @@
       <c r="B114" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="C114" s="8" t="s">
+      <c r="C114" s="9" t="s">
         <v>52</v>
       </c>
       <c r="E114" s="2" t="s">
@@ -2480,7 +2618,7 @@
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B115" s="5"/>
       <c r="C115" s="7"/>
-      <c r="E115" s="6" t="s">
+      <c r="E115" s="8" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2500,7 +2638,7 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B118" s="5"/>
-      <c r="C118" s="9" t="s">
+      <c r="C118" s="6" t="s">
         <v>54</v>
       </c>
       <c r="E118" t="s">
@@ -2557,7 +2695,7 @@
       <c r="B125" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C125" s="8" t="s">
+      <c r="C125" s="9" t="s">
         <v>52</v>
       </c>
       <c r="E125" s="2" t="s">
@@ -2567,7 +2705,7 @@
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B126" s="5"/>
       <c r="C126" s="7"/>
-      <c r="E126" s="6" t="s">
+      <c r="E126" s="8" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2587,7 +2725,7 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B129" s="5"/>
-      <c r="C129" s="9" t="s">
+      <c r="C129" s="6" t="s">
         <v>54</v>
       </c>
       <c r="E129" t="s">
@@ -2611,7 +2749,7 @@
       <c r="B133" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C133" s="8" t="s">
+      <c r="C133" s="9" t="s">
         <v>52</v>
       </c>
       <c r="E133" s="2" t="s">
@@ -2621,7 +2759,7 @@
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B134" s="5"/>
       <c r="C134" s="7"/>
-      <c r="E134" s="6" t="s">
+      <c r="E134" s="8" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2641,7 +2779,7 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B137" s="5"/>
-      <c r="C137" s="9" t="s">
+      <c r="C137" s="6" t="s">
         <v>54</v>
       </c>
       <c r="E137" t="s">
@@ -2698,7 +2836,7 @@
       <c r="B144" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="C144" s="8" t="s">
+      <c r="C144" s="9" t="s">
         <v>52</v>
       </c>
       <c r="E144" s="2" t="s">
@@ -2708,7 +2846,7 @@
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B145" s="5"/>
       <c r="C145" s="7"/>
-      <c r="E145" s="6" t="s">
+      <c r="E145" s="8" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2728,7 +2866,7 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B148" s="5"/>
-      <c r="C148" s="9" t="s">
+      <c r="C148" s="6" t="s">
         <v>54</v>
       </c>
       <c r="E148" t="s">
@@ -2752,7 +2890,7 @@
       <c r="B152" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="C152" s="8" t="s">
+      <c r="C152" s="9" t="s">
         <v>52</v>
       </c>
       <c r="E152" s="2" t="s">
@@ -2762,7 +2900,7 @@
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B153" s="5"/>
       <c r="C153" s="7"/>
-      <c r="E153" s="6" t="s">
+      <c r="E153" s="8" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2782,7 +2920,7 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B156" s="5"/>
-      <c r="C156" s="9" t="s">
+      <c r="C156" s="6" t="s">
         <v>54</v>
       </c>
       <c r="E156" t="s">
@@ -2801,50 +2939,32 @@
     </row>
   </sheetData>
   <mergeCells count="86">
-    <mergeCell ref="B144:B150"/>
-    <mergeCell ref="B152:B158"/>
-    <mergeCell ref="C156:C157"/>
-    <mergeCell ref="E153:E154"/>
-    <mergeCell ref="C148:C149"/>
-    <mergeCell ref="E145:E146"/>
-    <mergeCell ref="C152:C153"/>
-    <mergeCell ref="C154:C155"/>
-    <mergeCell ref="B64:B73"/>
-    <mergeCell ref="B75:B82"/>
-    <mergeCell ref="B84:B91"/>
-    <mergeCell ref="B94:B101"/>
-    <mergeCell ref="B55:B62"/>
-    <mergeCell ref="C144:C145"/>
-    <mergeCell ref="C146:C147"/>
-    <mergeCell ref="C129:C130"/>
-    <mergeCell ref="C114:C115"/>
-    <mergeCell ref="C116:C117"/>
-    <mergeCell ref="C118:C119"/>
-    <mergeCell ref="C133:C134"/>
-    <mergeCell ref="C135:C136"/>
-    <mergeCell ref="C137:C138"/>
-    <mergeCell ref="E134:E135"/>
-    <mergeCell ref="B103:B112"/>
-    <mergeCell ref="B114:B123"/>
-    <mergeCell ref="B125:B131"/>
-    <mergeCell ref="B133:B142"/>
-    <mergeCell ref="E115:E116"/>
-    <mergeCell ref="C125:C126"/>
-    <mergeCell ref="C127:C128"/>
-    <mergeCell ref="C98:C99"/>
-    <mergeCell ref="C100:C101"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="C103:C104"/>
-    <mergeCell ref="C105:C106"/>
-    <mergeCell ref="C107:C108"/>
-    <mergeCell ref="E104:E105"/>
-    <mergeCell ref="C96:C97"/>
-    <mergeCell ref="C84:C85"/>
-    <mergeCell ref="C86:C87"/>
-    <mergeCell ref="C88:C89"/>
-    <mergeCell ref="E85:E86"/>
-    <mergeCell ref="C94:C95"/>
-    <mergeCell ref="E95:E96"/>
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="B9:B15"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="B17:B24"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="B26:B32"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="C37:C38"/>
     <mergeCell ref="B35:B42"/>
     <mergeCell ref="C44:C45"/>
     <mergeCell ref="C46:C47"/>
@@ -2861,32 +2981,50 @@
     <mergeCell ref="C75:C76"/>
     <mergeCell ref="C77:C78"/>
     <mergeCell ref="B44:B53"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="B17:B24"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="B2:B7"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="B9:B15"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="B26:B32"/>
+    <mergeCell ref="C96:C97"/>
+    <mergeCell ref="C84:C85"/>
+    <mergeCell ref="C86:C87"/>
+    <mergeCell ref="C88:C89"/>
+    <mergeCell ref="E85:E86"/>
+    <mergeCell ref="C94:C95"/>
+    <mergeCell ref="E95:E96"/>
+    <mergeCell ref="C98:C99"/>
+    <mergeCell ref="C100:C101"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="C103:C104"/>
+    <mergeCell ref="C105:C106"/>
+    <mergeCell ref="C107:C108"/>
+    <mergeCell ref="E104:E105"/>
+    <mergeCell ref="C135:C136"/>
+    <mergeCell ref="C137:C138"/>
+    <mergeCell ref="E134:E135"/>
+    <mergeCell ref="B103:B112"/>
+    <mergeCell ref="B114:B123"/>
+    <mergeCell ref="B125:B131"/>
+    <mergeCell ref="B133:B142"/>
+    <mergeCell ref="E115:E116"/>
+    <mergeCell ref="C125:C126"/>
+    <mergeCell ref="C127:C128"/>
+    <mergeCell ref="C129:C130"/>
+    <mergeCell ref="C114:C115"/>
+    <mergeCell ref="C116:C117"/>
+    <mergeCell ref="C118:C119"/>
+    <mergeCell ref="C133:C134"/>
+    <mergeCell ref="B64:B73"/>
+    <mergeCell ref="B75:B82"/>
+    <mergeCell ref="B84:B91"/>
+    <mergeCell ref="B94:B101"/>
+    <mergeCell ref="B55:B62"/>
+    <mergeCell ref="B144:B150"/>
+    <mergeCell ref="B152:B158"/>
+    <mergeCell ref="C156:C157"/>
+    <mergeCell ref="E153:E154"/>
+    <mergeCell ref="C148:C149"/>
+    <mergeCell ref="E145:E146"/>
+    <mergeCell ref="C152:C153"/>
+    <mergeCell ref="C154:C155"/>
+    <mergeCell ref="C144:C145"/>
+    <mergeCell ref="C146:C147"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{889D356D-EDB0-E444-8DFA-AFB051D839AB}"/>
@@ -2909,4 +3047,1232 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3F649AE-22CA-DC47-B082-EB3DF4B64F93}">
+  <dimension ref="A1:I150"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D76" sqref="D76"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="60.6640625" customWidth="1"/>
+    <col min="3" max="3" width="56.5" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="5" max="5" width="75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B3" s="5"/>
+      <c r="C3" s="7"/>
+      <c r="E3" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B4" s="5"/>
+      <c r="C4" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B5" s="5"/>
+      <c r="C5" s="7"/>
+      <c r="E5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B6" s="5"/>
+      <c r="C6" s="6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B7" s="5"/>
+      <c r="C7" s="7"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B10" s="5"/>
+      <c r="C10" s="7"/>
+      <c r="E10" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B11" s="5"/>
+      <c r="C11" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B12" s="5"/>
+      <c r="C12" s="7"/>
+      <c r="E12" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B13" s="5"/>
+      <c r="C13" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B14" s="5"/>
+      <c r="C14" s="7"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B15" s="5"/>
+      <c r="C15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="5"/>
+      <c r="C18" s="7"/>
+      <c r="E18" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="5"/>
+      <c r="C19" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" s="7"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="5"/>
+      <c r="C20" s="7"/>
+      <c r="E20" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="5"/>
+      <c r="C21" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="5"/>
+      <c r="C22" s="7"/>
+      <c r="E22" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="5"/>
+      <c r="C23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B24" s="5"/>
+      <c r="C24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B27" s="5"/>
+      <c r="C27" s="7"/>
+      <c r="E27" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B28" s="5"/>
+      <c r="C28" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" s="7"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="5"/>
+      <c r="C29" s="7"/>
+      <c r="E29" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B30" s="5"/>
+      <c r="C30" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B31" s="5"/>
+      <c r="C31" s="7"/>
+      <c r="E31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B32" s="5"/>
+      <c r="C32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C33" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B36" s="5"/>
+      <c r="C36" s="7"/>
+      <c r="E36" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B37" s="5"/>
+      <c r="C37" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E37" s="7"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B38" s="5"/>
+      <c r="C38" s="7"/>
+      <c r="E38" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B39" s="5"/>
+      <c r="C39" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E39" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B40" s="5"/>
+      <c r="C40" s="7"/>
+      <c r="E40" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B41" s="5"/>
+      <c r="C41" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B42" s="5"/>
+      <c r="C42" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>78</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B45" s="5"/>
+      <c r="C45" s="7"/>
+      <c r="E45" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B46" s="5"/>
+      <c r="C46" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E46" s="7"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B47" s="5"/>
+      <c r="C47" s="7"/>
+      <c r="E47" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B48" s="5"/>
+      <c r="C48" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E48" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B49" s="5"/>
+      <c r="C49" s="7"/>
+      <c r="E49" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B50" s="5"/>
+      <c r="C50" t="s">
+        <v>73</v>
+      </c>
+      <c r="E50" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B51" s="5"/>
+      <c r="C51" t="s">
+        <v>80</v>
+      </c>
+      <c r="E51" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B52" s="5"/>
+      <c r="C52" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B53" s="5"/>
+      <c r="C53" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>85</v>
+      </c>
+      <c r="B55" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B56" s="11"/>
+      <c r="C56" s="7"/>
+      <c r="E56" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B57" s="11"/>
+      <c r="C57" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E57" s="7"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B58" s="11"/>
+      <c r="C58" s="7"/>
+      <c r="E58" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B59" s="11"/>
+      <c r="C59" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E59" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B60" s="11"/>
+      <c r="C60" s="7"/>
+      <c r="E60" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B61" s="11"/>
+      <c r="C61" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B62" s="11"/>
+      <c r="C62" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E63" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>90</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B65" s="5"/>
+      <c r="C65" s="7"/>
+      <c r="E65" s="7"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B66" s="5"/>
+      <c r="C66" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E66" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B67" s="5"/>
+      <c r="C67" s="7"/>
+      <c r="E67" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B68" s="5"/>
+      <c r="C68" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E68" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B69" s="5"/>
+      <c r="C69" s="7"/>
+      <c r="E69" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B70" s="5"/>
+      <c r="C70" t="s">
+        <v>73</v>
+      </c>
+      <c r="E70" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B71" s="5"/>
+      <c r="C71" t="s">
+        <v>80</v>
+      </c>
+      <c r="D71" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B72" s="5"/>
+      <c r="C72" t="s">
+        <v>81</v>
+      </c>
+      <c r="D72" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B73" s="5"/>
+      <c r="C73" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>94</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C75" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B76" s="5"/>
+      <c r="C76" s="7"/>
+      <c r="E76" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B77" s="5"/>
+      <c r="C77" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E77" s="7"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B78" s="5"/>
+      <c r="C78" s="7"/>
+      <c r="E78" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B79" s="5"/>
+      <c r="C79" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E79" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B80" s="5"/>
+      <c r="C80" s="7"/>
+      <c r="E80" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B81" s="5"/>
+      <c r="C81" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B82" s="5"/>
+      <c r="C82" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>23</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C84" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B85" s="5"/>
+      <c r="C85" s="7"/>
+      <c r="E85" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B86" s="5"/>
+      <c r="C86" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E86" s="7"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B87" s="5"/>
+      <c r="C87" s="7"/>
+      <c r="E87" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B88" s="5"/>
+      <c r="C88" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E88" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B89" s="5"/>
+      <c r="C89" s="7"/>
+      <c r="E89" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B90" s="5"/>
+      <c r="C90" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B91" s="5"/>
+      <c r="C91" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>24</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C94" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B95" s="5"/>
+      <c r="C95" s="7"/>
+      <c r="E95" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B96" s="5"/>
+      <c r="C96" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E96" s="7"/>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B97" s="5"/>
+      <c r="C97" s="7"/>
+      <c r="E97" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B98" s="5"/>
+      <c r="C98" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E98" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B99" s="5"/>
+      <c r="C99" s="7"/>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B100" s="5"/>
+      <c r="C100" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B101" s="5"/>
+      <c r="C101" s="7"/>
+    </row>
+    <row r="103" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>25</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C103" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B104" s="5"/>
+      <c r="C104" s="7"/>
+      <c r="E104" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B105" s="5"/>
+      <c r="C105" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E105" s="7"/>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B106" s="5"/>
+      <c r="C106" s="7"/>
+      <c r="E106" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B107" s="5"/>
+      <c r="C107" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="E107" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B108" s="5"/>
+      <c r="C108" s="7"/>
+      <c r="E108" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B109" s="5"/>
+      <c r="C109" t="s">
+        <v>104</v>
+      </c>
+      <c r="E109" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B110" s="5"/>
+      <c r="C110" t="s">
+        <v>105</v>
+      </c>
+      <c r="D110" t="s">
+        <v>152</v>
+      </c>
+      <c r="E110" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B111" s="5"/>
+      <c r="C111" t="s">
+        <v>106</v>
+      </c>
+      <c r="D111" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B112" s="5"/>
+      <c r="C112" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>114</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C114" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B115" s="5"/>
+      <c r="C115" s="7"/>
+      <c r="E115" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B116" s="5"/>
+      <c r="C116" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E116" s="7"/>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B117" s="5"/>
+      <c r="C117" s="7"/>
+      <c r="E117" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B118" s="5"/>
+      <c r="C118" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E118" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B119" s="5"/>
+      <c r="C119" s="7"/>
+      <c r="E119" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B120" s="5"/>
+      <c r="C120" t="s">
+        <v>104</v>
+      </c>
+      <c r="D120" t="s">
+        <v>152</v>
+      </c>
+      <c r="E120" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B121" s="5"/>
+      <c r="C121" t="s">
+        <v>105</v>
+      </c>
+      <c r="D121" t="s">
+        <v>109</v>
+      </c>
+      <c r="E121" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B122" s="5"/>
+      <c r="C122" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B123" s="5"/>
+      <c r="C123" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>117</v>
+      </c>
+      <c r="B125" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C125" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B126" s="5"/>
+      <c r="C126" s="7"/>
+      <c r="E126" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B127" s="5"/>
+      <c r="C127" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E127" s="7"/>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B128" s="5"/>
+      <c r="C128" s="7"/>
+      <c r="E128" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B129" s="5"/>
+      <c r="C129" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E129" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B130" s="5"/>
+      <c r="C130" s="7"/>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B131" s="5"/>
+      <c r="C131" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>120</v>
+      </c>
+      <c r="B133" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C133" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E133" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B134" s="5"/>
+      <c r="C134" s="7"/>
+      <c r="E134" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B135" s="5"/>
+      <c r="C135" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E135" s="7"/>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B136" s="5"/>
+      <c r="C136" s="7"/>
+      <c r="E136" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B137" s="5"/>
+      <c r="C137" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E137" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B138" s="5"/>
+      <c r="C138" s="7"/>
+      <c r="D138" t="s">
+        <v>152</v>
+      </c>
+      <c r="E138" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B139" s="5"/>
+      <c r="C139" t="s">
+        <v>73</v>
+      </c>
+      <c r="D139" t="s">
+        <v>146</v>
+      </c>
+      <c r="E139" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B140" s="5"/>
+      <c r="C140" t="s">
+        <v>121</v>
+      </c>
+      <c r="E140" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B141" s="5"/>
+      <c r="C141" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B142" s="5"/>
+      <c r="C142" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>126</v>
+      </c>
+      <c r="B144" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C144" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E144" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="145" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B145" s="5"/>
+      <c r="C145" s="7"/>
+      <c r="E145" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="146" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B146" s="5"/>
+      <c r="C146" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E146" s="7"/>
+    </row>
+    <row r="147" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B147" s="5"/>
+      <c r="C147" s="7"/>
+      <c r="E147" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="148" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B148" s="5"/>
+      <c r="C148" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E148" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="149" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B149" s="5"/>
+      <c r="C149" s="7"/>
+    </row>
+    <row r="150" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B150" s="5"/>
+      <c r="C150" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="81">
+    <mergeCell ref="B144:B150"/>
+    <mergeCell ref="C144:C145"/>
+    <mergeCell ref="E145:E146"/>
+    <mergeCell ref="C146:C147"/>
+    <mergeCell ref="C148:C149"/>
+    <mergeCell ref="B125:B131"/>
+    <mergeCell ref="C125:C126"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="C127:C128"/>
+    <mergeCell ref="C129:C130"/>
+    <mergeCell ref="B133:B142"/>
+    <mergeCell ref="C133:C134"/>
+    <mergeCell ref="E134:E135"/>
+    <mergeCell ref="C135:C136"/>
+    <mergeCell ref="C137:C138"/>
+    <mergeCell ref="B103:B112"/>
+    <mergeCell ref="C103:C104"/>
+    <mergeCell ref="E104:E105"/>
+    <mergeCell ref="C105:C106"/>
+    <mergeCell ref="C107:C108"/>
+    <mergeCell ref="B114:B123"/>
+    <mergeCell ref="C114:C115"/>
+    <mergeCell ref="E115:E116"/>
+    <mergeCell ref="C116:C117"/>
+    <mergeCell ref="C118:C119"/>
+    <mergeCell ref="B94:B101"/>
+    <mergeCell ref="C94:C95"/>
+    <mergeCell ref="E95:E96"/>
+    <mergeCell ref="C96:C97"/>
+    <mergeCell ref="C98:C99"/>
+    <mergeCell ref="C100:C101"/>
+    <mergeCell ref="B75:B82"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="E76:E77"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="B84:B91"/>
+    <mergeCell ref="C84:C85"/>
+    <mergeCell ref="E85:E86"/>
+    <mergeCell ref="C86:C87"/>
+    <mergeCell ref="C88:C89"/>
+    <mergeCell ref="B55:B62"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="B64:B73"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="E64:E65"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="B35:B42"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="B44:B53"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="B17:B24"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="B26:B32"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="B9:B15"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C13:C14"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{B08DFAAE-2FA6-7C41-A2B1-592513708D10}"/>
+    <hyperlink ref="C9" r:id="rId2" xr:uid="{50A28EC4-A3E7-F741-9B4D-1247AD1E1F6B}"/>
+    <hyperlink ref="C17" r:id="rId3" xr:uid="{B451E7FB-9CD7-214E-A3DA-01533AEE9006}"/>
+    <hyperlink ref="C26" r:id="rId4" xr:uid="{916B3F96-30A0-D04C-B60D-3B3197B5FF5F}"/>
+    <hyperlink ref="C35" r:id="rId5" xr:uid="{211A0A45-DF7E-DF4A-8EF6-AB69CBA85F02}"/>
+    <hyperlink ref="C44" r:id="rId6" xr:uid="{22E9308C-6471-EC4E-A654-7A454D0C29ED}"/>
+    <hyperlink ref="C55" r:id="rId7" xr:uid="{E9323948-87ED-7A4B-85EE-6E7078B1F64C}"/>
+    <hyperlink ref="C64" r:id="rId8" xr:uid="{77C120EE-E866-AA47-AF22-225A2B496B7F}"/>
+    <hyperlink ref="C75" r:id="rId9" xr:uid="{D0407355-7012-9A47-8E0C-F407895EA8B1}"/>
+    <hyperlink ref="C84" r:id="rId10" xr:uid="{28D997C4-2D5C-9742-83BB-1C298B8BB362}"/>
+    <hyperlink ref="C94" r:id="rId11" xr:uid="{E96F6AEC-4B6F-3F4F-A215-F4C5F240672E}"/>
+    <hyperlink ref="C103" r:id="rId12" xr:uid="{8EEA9A71-29ED-EC40-9E81-5967CA0D9DAB}"/>
+    <hyperlink ref="C114" r:id="rId13" xr:uid="{640FE8BE-94F6-A34A-9072-13A39E39F4BC}"/>
+    <hyperlink ref="C125" r:id="rId14" xr:uid="{3E078541-C505-0D47-8C68-DD2BDE09D1F3}"/>
+    <hyperlink ref="C133" r:id="rId15" xr:uid="{5C0FE46E-B15E-8945-B431-013BD4002AC2}"/>
+    <hyperlink ref="C144" r:id="rId16" xr:uid="{FF7DFA74-BF1F-5447-BB84-967F603B4C8F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>